<commit_message>
G2-918 Prevent redistribution of private code while satisfying the GPL work rules
</commit_message>
<xml_diff>
--- a/re-standard/src/main/java/com/g2forge/reassert/standard/model/contract/license/standardlicense.xlsx
+++ b/re-standard/src/main/java/com/g2forge/reassert/standard/model/contract/license/standardlicense.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\greg\g2forge\reassert\re-standard\src\main\java\com\g2forge\reassert\standard\model\contract\license\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD3F90D-55F3-4A8C-9E5E-E2BD77AEEF93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE686476-56E4-4B6C-86BF-B3CEFCB53583}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="33">
   <si>
     <t>contract</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>Zlib</t>
+  </si>
+  <si>
+    <t>NoRedistribution</t>
   </si>
 </sst>
 </file>
@@ -646,7 +649,17 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -989,10 +1002,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,7 +1018,7 @@
     <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1051,8 +1064,11 @@
       <c r="O1" t="s">
         <v>10</v>
       </c>
+      <c r="P1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1098,8 +1114,11 @@
       <c r="O2" t="s">
         <v>15</v>
       </c>
+      <c r="P2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1145,8 +1164,11 @@
       <c r="O3" t="s">
         <v>15</v>
       </c>
+      <c r="P3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1192,8 +1214,11 @@
       <c r="O4" t="s">
         <v>15</v>
       </c>
+      <c r="P4" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1239,8 +1264,11 @@
       <c r="O5" t="s">
         <v>15</v>
       </c>
+      <c r="P5" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1286,8 +1314,11 @@
       <c r="O6" t="s">
         <v>15</v>
       </c>
+      <c r="P6" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1333,8 +1364,11 @@
       <c r="O7" t="s">
         <v>15</v>
       </c>
+      <c r="P7" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1380,8 +1414,11 @@
       <c r="O8" t="s">
         <v>15</v>
       </c>
+      <c r="P8" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1427,8 +1464,11 @@
       <c r="O9" t="s">
         <v>15</v>
       </c>
+      <c r="P9" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1474,8 +1514,11 @@
       <c r="O10" t="s">
         <v>15</v>
       </c>
+      <c r="P10" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1521,8 +1564,11 @@
       <c r="O11" t="s">
         <v>15</v>
       </c>
+      <c r="P11" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1568,8 +1614,11 @@
       <c r="O12" t="s">
         <v>15</v>
       </c>
+      <c r="P12" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1615,8 +1664,11 @@
       <c r="O13" t="s">
         <v>15</v>
       </c>
+      <c r="P13" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1662,8 +1714,11 @@
       <c r="O14" t="s">
         <v>15</v>
       </c>
+      <c r="P14" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1709,8 +1764,11 @@
       <c r="O15" t="s">
         <v>16</v>
       </c>
+      <c r="P15" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1755,20 +1813,28 @@
       </c>
       <c r="O16" t="s">
         <v>15</v>
+      </c>
+      <c r="P16" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:F16">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"Included"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:K16">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Included"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:K16">
+  <conditionalFormatting sqref="L2:O16">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Included"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:O16">
+  <conditionalFormatting sqref="P2:P16">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Included"</formula>
     </cfRule>

</xml_diff>